<commit_message>
revised alliance classification for Epilobietea
</commit_message>
<xml_diff>
--- a/data/urban-sintaxa.xlsx
+++ b/data/urban-sintaxa.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unioviedo-my.sharepoint.com/personal/fernandezpeduardo_uniovi_es1/Documents/GitHub/manmade/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="314" documentId="13_ncr:1_{3441573B-DF2B-487A-8168-630E16E41485}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D086D9D2-53AF-461C-8FD2-3E9132D5119C}"/>
+  <xr:revisionPtr revIDLastSave="315" documentId="13_ncr:1_{3441573B-DF2B-487A-8168-630E16E41485}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0383A6E0-75FD-4B37-AD9C-755718A37827}"/>
   <bookViews>
-    <workbookView xWindow="40920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{3E21F8F6-C114-4632-89DF-E4FB12EA9A42}"/>
+    <workbookView xWindow="14235" yWindow="390" windowWidth="12420" windowHeight="15210" firstSheet="1" activeTab="2" xr2:uid="{3E21F8F6-C114-4632-89DF-E4FB12EA9A42}"/>
   </bookViews>
   <sheets>
     <sheet name="Sintaxones SIVIM" sheetId="2" r:id="rId1"/>
@@ -2235,12 +2235,12 @@
       <selection pane="bottomLeft" activeCell="A257" sqref="A257"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="70.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="70.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38.265625" customWidth="1"/>
+    <col min="1" max="1" width="38.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>303</v>
       </c>
@@ -2248,7 +2248,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="2" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>61</v>
       </c>
@@ -2256,7 +2256,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="3" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>98</v>
       </c>
@@ -2264,7 +2264,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="4" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>267</v>
       </c>
@@ -2272,7 +2272,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="5" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>98</v>
       </c>
@@ -2280,7 +2280,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="6" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>458</v>
       </c>
@@ -2288,7 +2288,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="7" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>359</v>
       </c>
@@ -2296,7 +2296,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="8" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>458</v>
       </c>
@@ -2304,7 +2304,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="9" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>458</v>
       </c>
@@ -2312,7 +2312,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="10" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>458</v>
       </c>
@@ -2320,7 +2320,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="11" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
         <v>399</v>
       </c>
@@ -2328,7 +2328,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="12" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>399</v>
       </c>
@@ -2336,7 +2336,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>399</v>
       </c>
@@ -2344,7 +2344,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>458</v>
       </c>
@@ -2352,7 +2352,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="15" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
         <v>399</v>
       </c>
@@ -2360,7 +2360,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>458</v>
       </c>
@@ -2368,7 +2368,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="17" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>458</v>
       </c>
@@ -2376,7 +2376,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="18" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
         <v>399</v>
       </c>
@@ -2384,7 +2384,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="19" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>458</v>
       </c>
@@ -2392,7 +2392,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="20" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>458</v>
       </c>
@@ -2400,7 +2400,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="21" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>458</v>
       </c>
@@ -2408,7 +2408,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="22" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>260</v>
       </c>
@@ -2416,7 +2416,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="23" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>260</v>
       </c>
@@ -2424,7 +2424,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="24" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>260</v>
       </c>
@@ -2432,7 +2432,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="25" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
         <v>399</v>
       </c>
@@ -2440,7 +2440,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="26" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="10" t="s">
         <v>399</v>
       </c>
@@ -2448,7 +2448,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="27" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>300</v>
       </c>
@@ -2456,7 +2456,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="28" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>458</v>
       </c>
@@ -2464,7 +2464,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="29" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>458</v>
       </c>
@@ -2472,7 +2472,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="30" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="s">
         <v>95</v>
       </c>
@@ -2480,7 +2480,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="31" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="10" t="s">
         <v>95</v>
       </c>
@@ -2488,7 +2488,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="32" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>307</v>
       </c>
@@ -2496,7 +2496,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="33" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="10" t="s">
         <v>95</v>
       </c>
@@ -2504,7 +2504,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="34" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="10" t="s">
         <v>95</v>
       </c>
@@ -2512,7 +2512,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="35" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>76</v>
       </c>
@@ -2520,7 +2520,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="36" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>277</v>
       </c>
@@ -2528,7 +2528,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="37" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>76</v>
       </c>
@@ -2536,7 +2536,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="38" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>76</v>
       </c>
@@ -2544,7 +2544,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="39" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>76</v>
       </c>
@@ -2552,7 +2552,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="40" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>76</v>
       </c>
@@ -2560,7 +2560,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="41" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>264</v>
       </c>
@@ -2568,7 +2568,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="42" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="10" t="s">
         <v>264</v>
       </c>
@@ -2576,7 +2576,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="43" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="10" t="s">
         <v>42</v>
       </c>
@@ -2584,7 +2584,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="44" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="10" t="s">
         <v>42</v>
       </c>
@@ -2592,7 +2592,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="45" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="10" t="s">
         <v>42</v>
       </c>
@@ -2600,7 +2600,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="46" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="10" t="s">
         <v>42</v>
       </c>
@@ -2608,7 +2608,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="47" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="10" t="s">
         <v>42</v>
       </c>
@@ -2616,7 +2616,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="48" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="10" t="s">
         <v>42</v>
       </c>
@@ -2624,7 +2624,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="49" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="10" t="s">
         <v>42</v>
       </c>
@@ -2632,7 +2632,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="50" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="10" t="s">
         <v>492</v>
       </c>
@@ -2640,7 +2640,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="51" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="10" t="s">
         <v>42</v>
       </c>
@@ -2648,7 +2648,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="52" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="10" t="s">
         <v>492</v>
       </c>
@@ -2656,7 +2656,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="53" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="10" t="s">
         <v>42</v>
       </c>
@@ -2664,7 +2664,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="54" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="10" t="s">
         <v>42</v>
       </c>
@@ -2672,7 +2672,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="55" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="10" t="s">
         <v>42</v>
       </c>
@@ -2680,7 +2680,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="56" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="10" t="s">
         <v>399</v>
       </c>
@@ -2688,7 +2688,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="57" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
         <v>88</v>
       </c>
@@ -2696,7 +2696,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="58" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="10" t="s">
         <v>42</v>
       </c>
@@ -2704,7 +2704,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="59" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="10" t="s">
         <v>42</v>
       </c>
@@ -2712,7 +2712,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="60" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="10" t="s">
         <v>42</v>
       </c>
@@ -2720,7 +2720,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="61" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="10" t="s">
         <v>42</v>
       </c>
@@ -2728,7 +2728,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="62" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
         <v>88</v>
       </c>
@@ -2736,7 +2736,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="63" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="10" t="s">
         <v>42</v>
       </c>
@@ -2744,7 +2744,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="64" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="10" t="s">
         <v>42</v>
       </c>
@@ -2752,7 +2752,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="65" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="10" t="s">
         <v>42</v>
       </c>
@@ -2760,7 +2760,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="66" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="10" t="s">
         <v>42</v>
       </c>
@@ -2768,7 +2768,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="67" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="10" t="s">
         <v>42</v>
       </c>
@@ -2776,7 +2776,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="68" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="10" t="s">
         <v>42</v>
       </c>
@@ -2784,7 +2784,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="69" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" s="10" t="s">
         <v>42</v>
       </c>
@@ -2792,7 +2792,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="70" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>13</v>
       </c>
@@ -2800,7 +2800,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="71" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>13</v>
       </c>
@@ -2808,7 +2808,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="72" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="10" t="s">
         <v>42</v>
       </c>
@@ -2816,7 +2816,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="73" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" s="10" t="s">
         <v>42</v>
       </c>
@@ -2824,7 +2824,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="74" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" s="10" t="s">
         <v>42</v>
       </c>
@@ -2832,7 +2832,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="75" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" s="10" t="s">
         <v>42</v>
       </c>
@@ -2840,7 +2840,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="76" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" s="10" t="s">
         <v>24</v>
       </c>
@@ -2848,7 +2848,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="77" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" s="10" t="s">
         <v>24</v>
       </c>
@@ -2856,7 +2856,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="78" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" s="10" t="s">
         <v>24</v>
       </c>
@@ -2864,7 +2864,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="79" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" s="10" t="s">
         <v>277</v>
       </c>
@@ -2872,7 +2872,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="80" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" s="10" t="s">
         <v>24</v>
       </c>
@@ -2880,7 +2880,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="81" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>40</v>
       </c>
@@ -2888,7 +2888,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="82" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" s="4" t="s">
         <v>285</v>
       </c>
@@ -2896,7 +2896,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="83" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>333</v>
       </c>
@@ -2904,7 +2904,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="84" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" s="4" t="s">
         <v>326</v>
       </c>
@@ -2912,7 +2912,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="85" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" s="4" t="s">
         <v>326</v>
       </c>
@@ -2920,7 +2920,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="86" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" s="6" t="s">
         <v>88</v>
       </c>
@@ -2928,7 +2928,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="87" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" s="6" t="s">
         <v>88</v>
       </c>
@@ -2936,7 +2936,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="88" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" s="6" t="s">
         <v>88</v>
       </c>
@@ -2944,7 +2944,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="89" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" s="6" t="s">
         <v>88</v>
       </c>
@@ -2952,7 +2952,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="90" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" s="6" t="s">
         <v>88</v>
       </c>
@@ -2960,7 +2960,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="91" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" s="10" t="s">
         <v>326</v>
       </c>
@@ -2968,7 +2968,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="92" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" s="10" t="s">
         <v>326</v>
       </c>
@@ -2976,7 +2976,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="93" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" s="10" t="s">
         <v>326</v>
       </c>
@@ -2984,7 +2984,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="94" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" s="10" t="s">
         <v>326</v>
       </c>
@@ -2992,7 +2992,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="95" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>92</v>
       </c>
@@ -3000,7 +3000,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="96" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>92</v>
       </c>
@@ -3008,7 +3008,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="97" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>92</v>
       </c>
@@ -3016,7 +3016,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="98" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
         <v>312</v>
       </c>
@@ -3024,7 +3024,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="99" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" s="5" t="s">
         <v>293</v>
       </c>
@@ -3032,7 +3032,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="100" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" s="5" t="s">
         <v>293</v>
       </c>
@@ -3040,7 +3040,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="101" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>92</v>
       </c>
@@ -3048,7 +3048,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="102" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>92</v>
       </c>
@@ -3056,7 +3056,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="103" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>92</v>
       </c>
@@ -3064,7 +3064,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="104" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>92</v>
       </c>
@@ -3072,7 +3072,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="105" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>92</v>
       </c>
@@ -3080,7 +3080,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="106" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" s="3" t="s">
         <v>289</v>
       </c>
@@ -3088,7 +3088,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="107" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" s="4" t="s">
         <v>320</v>
       </c>
@@ -3096,7 +3096,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="108" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" s="4" t="s">
         <v>59</v>
       </c>
@@ -3104,7 +3104,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="109" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
         <v>331</v>
       </c>
@@ -3112,7 +3112,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="110" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" s="4" t="s">
         <v>287</v>
       </c>
@@ -3120,7 +3120,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="111" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
         <v>40</v>
       </c>
@@ -3128,7 +3128,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="112" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
         <v>310</v>
       </c>
@@ -3136,7 +3136,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="113" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
         <v>40</v>
       </c>
@@ -3144,7 +3144,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="114" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" s="4" t="s">
         <v>280</v>
       </c>
@@ -3152,7 +3152,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="115" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
         <v>362</v>
       </c>
@@ -3160,7 +3160,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="116" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>92</v>
       </c>
@@ -3168,7 +3168,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="117" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
         <v>40</v>
       </c>
@@ -3176,7 +3176,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="118" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" s="6" t="s">
         <v>389</v>
       </c>
@@ -3184,7 +3184,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="119" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
         <v>75</v>
       </c>
@@ -3192,7 +3192,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="120" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="120" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
         <v>75</v>
       </c>
@@ -3200,7 +3200,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="121" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="121" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
         <v>75</v>
       </c>
@@ -3208,7 +3208,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="122" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
         <v>330</v>
       </c>
@@ -3216,7 +3216,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="123" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="123" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
         <v>271</v>
       </c>
@@ -3224,7 +3224,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="124" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="124" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
         <v>271</v>
       </c>
@@ -3232,7 +3232,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="125" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="125" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
         <v>271</v>
       </c>
@@ -3240,7 +3240,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="126" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="126" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
         <v>271</v>
       </c>
@@ -3248,7 +3248,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="127" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="127" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
         <v>55</v>
       </c>
@@ -3256,7 +3256,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="128" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="128" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
         <v>491</v>
       </c>
@@ -3264,7 +3264,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="129" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="129" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" s="3" t="s">
         <v>229</v>
       </c>
@@ -3272,7 +3272,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="130" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="130" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
         <v>55</v>
       </c>
@@ -3280,7 +3280,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="131" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="131" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
         <v>55</v>
       </c>
@@ -3288,7 +3288,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="132" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="132" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
         <v>55</v>
       </c>
@@ -3296,7 +3296,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="133" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="133" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133" s="10" t="s">
         <v>487</v>
       </c>
@@ -3304,7 +3304,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="134" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="134" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" s="4" t="s">
         <v>323</v>
       </c>
@@ -3312,7 +3312,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="135" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="135" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135" s="4" t="s">
         <v>323</v>
       </c>
@@ -3320,7 +3320,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="136" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="136" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" s="18" t="s">
         <v>486</v>
       </c>
@@ -3328,7 +3328,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="137" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="137" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
         <v>296</v>
       </c>
@@ -3336,7 +3336,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="138" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="138" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138" s="10" t="s">
         <v>109</v>
       </c>
@@ -3344,7 +3344,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="139" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="139" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139" s="10" t="s">
         <v>109</v>
       </c>
@@ -3352,7 +3352,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="140" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="140" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140" s="18" t="s">
         <v>486</v>
       </c>
@@ -3360,7 +3360,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="141" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="141" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141" s="18" t="s">
         <v>486</v>
       </c>
@@ -3368,7 +3368,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="142" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="142" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142" s="10" t="s">
         <v>487</v>
       </c>
@@ -3376,7 +3376,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="143" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="143" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143" s="4" t="s">
         <v>364</v>
       </c>
@@ -3384,7 +3384,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="144" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="144" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144" s="4" t="s">
         <v>364</v>
       </c>
@@ -3392,7 +3392,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="145" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="145" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145" s="3" t="s">
         <v>316</v>
       </c>
@@ -3400,7 +3400,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="146" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="146" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146" s="10" t="s">
         <v>487</v>
       </c>
@@ -3408,7 +3408,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="147" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="147" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147" s="10" t="s">
         <v>487</v>
       </c>
@@ -3416,7 +3416,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="148" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="148" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148" s="10" t="s">
         <v>487</v>
       </c>
@@ -3424,7 +3424,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="149" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="149" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149" s="18" t="s">
         <v>486</v>
       </c>
@@ -3432,7 +3432,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="150" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="150" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150" s="3" t="s">
         <v>488</v>
       </c>
@@ -3440,7 +3440,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="151" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="151" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151" s="3" t="s">
         <v>488</v>
       </c>
@@ -3448,7 +3448,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="152" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="152" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152" s="3" t="s">
         <v>83</v>
       </c>
@@ -3456,7 +3456,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="153" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="153" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153" s="3" t="s">
         <v>83</v>
       </c>
@@ -3464,7 +3464,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="154" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="154" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154" s="3" t="s">
         <v>83</v>
       </c>
@@ -3472,7 +3472,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="155" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="155" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155" s="3" t="s">
         <v>83</v>
       </c>
@@ -3480,7 +3480,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="156" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="156" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156" s="3" t="s">
         <v>83</v>
       </c>
@@ -3488,7 +3488,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="157" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157" s="3" t="s">
         <v>83</v>
       </c>
@@ -3496,7 +3496,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="158" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="158" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
         <v>310</v>
       </c>
@@ -3504,7 +3504,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="159" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="159" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159" s="10" t="s">
         <v>100</v>
       </c>
@@ -3512,7 +3512,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="160" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="160" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
         <v>91</v>
       </c>
@@ -3520,7 +3520,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="161" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="161" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161" s="10" t="s">
         <v>69</v>
       </c>
@@ -3528,7 +3528,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="162" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="162" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162" s="10" t="s">
         <v>69</v>
       </c>
@@ -3536,7 +3536,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="163" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="163" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163" s="10" t="s">
         <v>69</v>
       </c>
@@ -3544,7 +3544,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="164" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="164" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164" s="10" t="s">
         <v>69</v>
       </c>
@@ -3552,7 +3552,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="165" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="165" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165" s="1" t="s">
         <v>72</v>
       </c>
@@ -3560,7 +3560,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="166" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="166" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
         <v>72</v>
       </c>
@@ -3568,7 +3568,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="167" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="167" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167" s="1" t="s">
         <v>267</v>
       </c>
@@ -3576,7 +3576,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="168" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="168" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168" s="3" t="s">
         <v>87</v>
       </c>
@@ -3584,7 +3584,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="169" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="169" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169" s="3" t="s">
         <v>87</v>
       </c>
@@ -3592,7 +3592,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="170" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="170" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170" s="3" t="s">
         <v>87</v>
       </c>
@@ -3600,7 +3600,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="171" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="171" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171" s="10" t="s">
         <v>39</v>
       </c>
@@ -3608,7 +3608,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="172" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="172" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172" s="10" t="s">
         <v>39</v>
       </c>
@@ -3616,7 +3616,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="173" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="173" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173" s="10" t="s">
         <v>39</v>
       </c>
@@ -3624,7 +3624,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="174" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="174" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174" s="10" t="s">
         <v>39</v>
       </c>
@@ -3632,7 +3632,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="175" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="175" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A175" s="4" t="s">
         <v>261</v>
       </c>
@@ -3640,7 +3640,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="176" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="176" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176" s="4" t="s">
         <v>261</v>
       </c>
@@ -3648,7 +3648,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="177" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="177" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177" s="3" t="s">
         <v>274</v>
       </c>
@@ -3656,7 +3656,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="178" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="178" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A178" s="3" t="s">
         <v>274</v>
       </c>
@@ -3664,7 +3664,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="179" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="179" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A179" s="10" t="s">
         <v>39</v>
       </c>
@@ -3672,7 +3672,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="180" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="180" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180" s="10" t="s">
         <v>39</v>
       </c>
@@ -3680,7 +3680,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="181" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="181" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A181" s="1" t="s">
         <v>31</v>
       </c>
@@ -3688,7 +3688,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="182" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="182" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182" s="1" t="s">
         <v>31</v>
       </c>
@@ -3696,7 +3696,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="183" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="183" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A183" s="1" t="s">
         <v>31</v>
       </c>
@@ -3704,7 +3704,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="184" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="184" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A184" s="1" t="s">
         <v>31</v>
       </c>
@@ -3712,7 +3712,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="185" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="185" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185" s="1" t="s">
         <v>31</v>
       </c>
@@ -3720,7 +3720,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="186" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="186" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A186" s="1" t="s">
         <v>283</v>
       </c>
@@ -3728,7 +3728,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="187" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="187" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A187" s="1" t="s">
         <v>283</v>
       </c>
@@ -3736,7 +3736,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="188" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="188" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A188" s="10" t="s">
         <v>20</v>
       </c>
@@ -3744,7 +3744,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="189" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="189" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A189" s="10" t="s">
         <v>20</v>
       </c>
@@ -3752,7 +3752,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="190" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="190" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A190" s="1" t="s">
         <v>36</v>
       </c>
@@ -3760,7 +3760,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="191" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="191" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A191" s="1" t="s">
         <v>36</v>
       </c>
@@ -3768,7 +3768,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="192" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="192" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A192" s="1" t="s">
         <v>36</v>
       </c>
@@ -3776,7 +3776,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="193" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="193" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A193" s="1" t="s">
         <v>36</v>
       </c>
@@ -3784,7 +3784,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="194" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="194" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A194" s="1" t="s">
         <v>109</v>
       </c>
@@ -3792,7 +3792,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="195" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="195" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A195" s="1" t="s">
         <v>109</v>
       </c>
@@ -3800,7 +3800,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="196" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="196" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A196" s="1" t="s">
         <v>67</v>
       </c>
@@ -3808,7 +3808,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="197" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="197" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A197" s="1" t="s">
         <v>67</v>
       </c>
@@ -3816,7 +3816,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="198" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="198" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A198" s="1" t="s">
         <v>67</v>
       </c>
@@ -3824,7 +3824,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="199" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="199" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A199" s="1" t="s">
         <v>67</v>
       </c>
@@ -3832,7 +3832,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="200" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="200" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A200" s="1" t="s">
         <v>67</v>
       </c>
@@ -3840,7 +3840,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="201" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="201" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A201" s="1" t="s">
         <v>67</v>
       </c>
@@ -3848,7 +3848,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="202" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="202" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A202" s="1" t="s">
         <v>67</v>
       </c>
@@ -3856,7 +3856,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="203" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="203" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A203" s="1" t="s">
         <v>67</v>
       </c>
@@ -3864,7 +3864,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="204" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="204" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A204" s="1" t="s">
         <v>67</v>
       </c>
@@ -3872,7 +3872,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="205" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="205" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A205" s="1" t="s">
         <v>109</v>
       </c>
@@ -3880,7 +3880,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="206" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="206" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A206" s="1" t="s">
         <v>67</v>
       </c>
@@ -3888,7 +3888,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="207" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="207" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A207" s="1" t="s">
         <v>67</v>
       </c>
@@ -3896,7 +3896,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="208" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="208" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A208" s="1" t="s">
         <v>67</v>
       </c>
@@ -3904,7 +3904,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="209" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="209" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A209" s="1" t="s">
         <v>292</v>
       </c>
@@ -3912,7 +3912,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="210" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="210" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A210" s="1" t="s">
         <v>50</v>
       </c>
@@ -3920,7 +3920,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="211" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="211" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A211" s="4" t="s">
         <v>240</v>
       </c>
@@ -3928,7 +3928,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="212" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="212" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A212" s="4" t="s">
         <v>240</v>
       </c>
@@ -3936,7 +3936,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="213" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="213" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A213" s="4" t="s">
         <v>240</v>
       </c>
@@ -3944,7 +3944,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="214" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="214" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A214" s="4" t="s">
         <v>240</v>
       </c>
@@ -3952,7 +3952,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="215" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="215" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A215" s="4" t="s">
         <v>240</v>
       </c>
@@ -3960,7 +3960,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="216" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="216" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A216" s="4" t="s">
         <v>240</v>
       </c>
@@ -3968,7 +3968,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="217" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="217" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A217" s="5" t="s">
         <v>317</v>
       </c>
@@ -3976,7 +3976,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="218" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="218" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A218" s="5" t="s">
         <v>317</v>
       </c>
@@ -3984,7 +3984,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="219" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="219" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A219" s="5" t="s">
         <v>327</v>
       </c>
@@ -3992,7 +3992,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="220" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="220" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A220" s="5" t="s">
         <v>327</v>
       </c>
@@ -4000,7 +4000,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="221" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="221" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A221" s="1" t="s">
         <v>50</v>
       </c>
@@ -4008,7 +4008,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="222" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="222" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A222" s="4" t="s">
         <v>272</v>
       </c>
@@ -4016,7 +4016,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="223" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="223" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A223" s="5" t="s">
         <v>358</v>
       </c>
@@ -4024,7 +4024,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="224" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="224" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A224" s="4" t="s">
         <v>370</v>
       </c>
@@ -4032,7 +4032,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="225" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="225" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>267</v>
       </c>
@@ -4040,7 +4040,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="226" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="226" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A226" s="1" t="s">
         <v>398</v>
       </c>
@@ -4048,7 +4048,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="227" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="227" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A227" s="1" t="s">
         <v>36</v>
       </c>
@@ -4056,7 +4056,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="228" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="228" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>36</v>
       </c>
@@ -4064,7 +4064,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="229" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="229" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>72</v>
       </c>
@@ -4072,7 +4072,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="230" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="230" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>72</v>
       </c>
@@ -4080,7 +4080,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="231" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="231" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>456</v>
       </c>
@@ -4088,7 +4088,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="232" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="232" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>13</v>
       </c>
@@ -4096,7 +4096,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="233" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="233" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>437</v>
       </c>
@@ -4104,7 +4104,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="234" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="234" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>320</v>
       </c>
@@ -4112,7 +4112,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="235" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="235" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>59</v>
       </c>
@@ -4120,7 +4120,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="236" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="236" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>59</v>
       </c>
@@ -4128,7 +4128,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="237" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="237" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>59</v>
       </c>
@@ -4136,7 +4136,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="238" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="238" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>59</v>
       </c>
@@ -4144,7 +4144,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="239" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="239" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>433</v>
       </c>
@@ -4152,7 +4152,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="240" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="240" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>397</v>
       </c>
@@ -4160,7 +4160,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="241" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="241" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>397</v>
       </c>
@@ -4168,7 +4168,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="242" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="242" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>326</v>
       </c>
@@ -4176,7 +4176,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="243" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="243" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>438</v>
       </c>
@@ -4184,7 +4184,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="244" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="244" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>439</v>
       </c>
@@ -4192,7 +4192,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="245" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="245" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>434</v>
       </c>
@@ -4200,7 +4200,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="246" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="246" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>296</v>
       </c>
@@ -4208,7 +4208,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="247" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="247" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>435</v>
       </c>
@@ -4216,7 +4216,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="248" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="248" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>436</v>
       </c>
@@ -4224,7 +4224,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="249" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="249" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>261</v>
       </c>
@@ -4232,7 +4232,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="250" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="250" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>570</v>
       </c>
@@ -4240,7 +4240,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="251" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="251" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>61</v>
       </c>
@@ -4248,7 +4248,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="252" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="252" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>326</v>
       </c>
@@ -4256,7 +4256,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="253" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="253" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>36</v>
       </c>
@@ -4264,7 +4264,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="254" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="254" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>570</v>
       </c>
@@ -4297,24 +4297,24 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:I82"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C86" sqref="C86"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F77" sqref="F77"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="70.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="70.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.59765625" customWidth="1"/>
-    <col min="2" max="2" width="10.59765625" customWidth="1"/>
-    <col min="3" max="3" width="41.59765625" customWidth="1"/>
-    <col min="4" max="4" width="31.73046875" customWidth="1"/>
-    <col min="5" max="5" width="43.73046875" customWidth="1"/>
-    <col min="6" max="6" width="38.73046875" customWidth="1"/>
-    <col min="7" max="7" width="20.3984375" customWidth="1"/>
-    <col min="8" max="8" width="19.59765625" customWidth="1"/>
-    <col min="9" max="9" width="10.86328125" customWidth="1"/>
+    <col min="1" max="1" width="14.5703125" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" customWidth="1"/>
+    <col min="3" max="3" width="41.5703125" customWidth="1"/>
+    <col min="4" max="4" width="31.7109375" customWidth="1"/>
+    <col min="5" max="5" width="43.7109375" customWidth="1"/>
+    <col min="6" max="6" width="38.7109375" customWidth="1"/>
+    <col min="7" max="7" width="20.42578125" customWidth="1"/>
+    <col min="8" max="8" width="19.5703125" customWidth="1"/>
+    <col min="9" max="9" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>405</v>
       </c>
@@ -4343,7 +4343,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="2" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>338</v>
       </c>
@@ -4372,7 +4372,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="3" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>338</v>
       </c>
@@ -4401,7 +4401,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="4" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>338</v>
       </c>
@@ -4424,7 +4424,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="5" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
         <v>338</v>
       </c>
@@ -4453,7 +4453,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="6" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
         <v>338</v>
       </c>
@@ -4482,7 +4482,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="7" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
         <v>338</v>
       </c>
@@ -4511,7 +4511,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="8" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>337</v>
       </c>
@@ -4532,7 +4532,7 @@
       </c>
       <c r="G8" s="13"/>
     </row>
-    <row r="9" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>337</v>
       </c>
@@ -4553,7 +4553,7 @@
       </c>
       <c r="G9" s="12"/>
     </row>
-    <row r="10" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>337</v>
       </c>
@@ -4574,7 +4574,7 @@
       </c>
       <c r="G10" s="12"/>
     </row>
-    <row r="11" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>337</v>
       </c>
@@ -4595,7 +4595,7 @@
       </c>
       <c r="G11" s="12"/>
     </row>
-    <row r="12" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>337</v>
       </c>
@@ -4616,7 +4616,7 @@
       </c>
       <c r="G12" s="12"/>
     </row>
-    <row r="13" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
         <v>337</v>
       </c>
@@ -4637,7 +4637,7 @@
       </c>
       <c r="G13" s="12"/>
     </row>
-    <row r="14" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
         <v>337</v>
       </c>
@@ -4658,7 +4658,7 @@
       </c>
       <c r="G14" s="12"/>
     </row>
-    <row r="15" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>337</v>
       </c>
@@ -4679,7 +4679,7 @@
       </c>
       <c r="G15" s="12"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>337</v>
       </c>
@@ -4700,7 +4700,7 @@
       </c>
       <c r="G16" s="12"/>
     </row>
-    <row r="17" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>337</v>
       </c>
@@ -4721,7 +4721,7 @@
       </c>
       <c r="G17" s="12"/>
     </row>
-    <row r="18" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>337</v>
       </c>
@@ -4744,7 +4744,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="19" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>337</v>
       </c>
@@ -4765,7 +4765,7 @@
       </c>
       <c r="G19" s="12"/>
     </row>
-    <row r="20" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>337</v>
       </c>
@@ -4786,7 +4786,7 @@
       </c>
       <c r="G20" s="12"/>
     </row>
-    <row r="21" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>337</v>
       </c>
@@ -4807,7 +4807,7 @@
       </c>
       <c r="G21" s="12"/>
     </row>
-    <row r="22" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>337</v>
       </c>
@@ -4828,7 +4828,7 @@
       </c>
       <c r="G22" s="12"/>
     </row>
-    <row r="23" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>337</v>
       </c>
@@ -4849,7 +4849,7 @@
       </c>
       <c r="G23" s="12"/>
     </row>
-    <row r="24" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>337</v>
       </c>
@@ -4870,7 +4870,7 @@
       </c>
       <c r="G24" s="12"/>
     </row>
-    <row r="25" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="14" t="s">
         <v>337</v>
       </c>
@@ -4891,7 +4891,7 @@
       </c>
       <c r="G25" s="12"/>
     </row>
-    <row r="26" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>337</v>
       </c>
@@ -4912,7 +4912,7 @@
       </c>
       <c r="G26" s="12"/>
     </row>
-    <row r="27" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>337</v>
       </c>
@@ -4933,7 +4933,7 @@
       </c>
       <c r="G27" s="12"/>
     </row>
-    <row r="28" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>337</v>
       </c>
@@ -4954,7 +4954,7 @@
       </c>
       <c r="G28" s="12"/>
     </row>
-    <row r="29" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>337</v>
       </c>
@@ -4975,7 +4975,7 @@
       </c>
       <c r="G29" s="12"/>
     </row>
-    <row r="30" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>337</v>
       </c>
@@ -4996,7 +4996,7 @@
       </c>
       <c r="G30" s="12"/>
     </row>
-    <row r="31" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>337</v>
       </c>
@@ -5017,7 +5017,7 @@
       </c>
       <c r="G31" s="12"/>
     </row>
-    <row r="32" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>337</v>
       </c>
@@ -5038,7 +5038,7 @@
       </c>
       <c r="G32" s="12"/>
     </row>
-    <row r="33" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="14" t="s">
         <v>337</v>
       </c>
@@ -5059,7 +5059,7 @@
       </c>
       <c r="G33" s="12"/>
     </row>
-    <row r="34" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>337</v>
       </c>
@@ -5080,7 +5080,7 @@
       </c>
       <c r="G34" s="12"/>
     </row>
-    <row r="35" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>337</v>
       </c>
@@ -5101,7 +5101,7 @@
       </c>
       <c r="G35" s="12"/>
     </row>
-    <row r="36" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>337</v>
       </c>
@@ -5122,7 +5122,7 @@
       </c>
       <c r="G36" s="12"/>
     </row>
-    <row r="37" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="18" t="s">
         <v>338</v>
       </c>
@@ -5151,7 +5151,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="38" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
         <v>338</v>
       </c>
@@ -5174,7 +5174,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="39" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
         <v>338</v>
       </c>
@@ -5197,7 +5197,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="40" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="18" t="s">
         <v>338</v>
       </c>
@@ -5226,7 +5226,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="41" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
         <v>338</v>
       </c>
@@ -5249,7 +5249,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="42" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="18" t="s">
         <v>338</v>
       </c>
@@ -5278,7 +5278,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="43" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="18" t="s">
         <v>338</v>
       </c>
@@ -5307,7 +5307,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="44" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="18" t="s">
         <v>338</v>
       </c>
@@ -5336,7 +5336,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="45" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
         <v>338</v>
       </c>
@@ -5357,7 +5357,7 @@
       </c>
       <c r="G45" s="9"/>
     </row>
-    <row r="46" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="18" t="s">
         <v>338</v>
       </c>
@@ -5386,7 +5386,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="47" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="18" t="s">
         <v>338</v>
       </c>
@@ -5415,7 +5415,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="48" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="7" t="s">
         <v>338</v>
       </c>
@@ -5438,7 +5438,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="49" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
         <v>338</v>
       </c>
@@ -5464,7 +5464,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="50" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="18" t="s">
         <v>338</v>
       </c>
@@ -5493,7 +5493,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="51" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="18" t="s">
         <v>338</v>
       </c>
@@ -5522,7 +5522,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="52" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="7" t="s">
         <v>338</v>
       </c>
@@ -5545,7 +5545,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="53" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="18" t="s">
         <v>338</v>
       </c>
@@ -5574,7 +5574,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="54" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="7" t="s">
         <v>338</v>
       </c>
@@ -5597,7 +5597,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="55" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="18" t="s">
         <v>338</v>
       </c>
@@ -5626,7 +5626,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="56" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="18" t="s">
         <v>338</v>
       </c>
@@ -5655,7 +5655,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="57" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
         <v>337</v>
       </c>
@@ -5681,7 +5681,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="58" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="18" t="s">
         <v>338</v>
       </c>
@@ -5710,7 +5710,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="59" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="18" t="s">
         <v>338</v>
       </c>
@@ -5739,7 +5739,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="60" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
         <v>337</v>
       </c>
@@ -5765,7 +5765,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="61" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="7" t="s">
         <v>338</v>
       </c>
@@ -5788,7 +5788,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="62" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="16" t="s">
         <v>337</v>
       </c>
@@ -5811,7 +5811,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="63" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="18" t="s">
         <v>338</v>
       </c>
@@ -5840,7 +5840,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="64" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="18" t="s">
         <v>338</v>
       </c>
@@ -5869,7 +5869,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="65" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="18" t="s">
         <v>338</v>
       </c>
@@ -5898,7 +5898,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="66" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="7" t="s">
         <v>338</v>
       </c>
@@ -5921,7 +5921,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="67" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="18" t="s">
         <v>338</v>
       </c>
@@ -5950,7 +5950,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="68" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="18" t="s">
         <v>338</v>
       </c>
@@ -5979,7 +5979,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="69" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>337</v>
       </c>
@@ -5999,7 +5999,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="70" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>337</v>
       </c>
@@ -6019,7 +6019,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="71" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>337</v>
       </c>
@@ -6039,7 +6039,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="72" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>337</v>
       </c>
@@ -6059,7 +6059,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="73" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>337</v>
       </c>
@@ -6079,7 +6079,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="74" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>337</v>
       </c>
@@ -6099,7 +6099,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="75" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>337</v>
       </c>
@@ -6119,7 +6119,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="76" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>337</v>
       </c>
@@ -6139,7 +6139,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="77" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" s="18" t="s">
         <v>338</v>
       </c>
@@ -6168,7 +6168,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="78" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" s="7" t="s">
         <v>338</v>
       </c>
@@ -6191,7 +6191,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="79" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" s="4" t="s">
         <v>337</v>
       </c>
@@ -6214,7 +6214,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="80" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" s="18" t="s">
         <v>337</v>
       </c>
@@ -6234,7 +6234,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="81" spans="1:7" hidden="1" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" s="18" t="s">
         <v>338</v>
       </c>
@@ -6257,7 +6257,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" s="4" t="s">
         <v>337</v>
       </c>
@@ -6281,7 +6281,7 @@
   <autoFilter ref="A1:H82" xr:uid="{CD16DA9A-CBD5-4A81-9BAB-93F15106FEF8}">
     <filterColumn colId="3">
       <filters>
-        <filter val="Juncetea maritimi"/>
+        <filter val="Epilobietea angustifolii"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -6300,18 +6300,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5D13668-5AFE-4B9C-AD33-502416580960}">
   <dimension ref="A1:C65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B46" sqref="B46"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.1328125" customWidth="1"/>
-    <col min="2" max="2" width="59.265625" customWidth="1"/>
-    <col min="3" max="3" width="92.265625" customWidth="1"/>
+    <col min="1" max="1" width="39.140625" customWidth="1"/>
+    <col min="2" max="2" width="59.28515625" customWidth="1"/>
+    <col min="3" max="3" width="92.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>303</v>
       </c>
@@ -6322,7 +6322,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>50</v>
       </c>
@@ -6333,7 +6333,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>50</v>
       </c>
@@ -6344,7 +6344,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>486</v>
       </c>
@@ -6355,7 +6355,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>486</v>
       </c>
@@ -6366,7 +6366,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>486</v>
       </c>
@@ -6377,7 +6377,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>67</v>
       </c>
@@ -6388,7 +6388,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>67</v>
       </c>
@@ -6399,7 +6399,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>67</v>
       </c>
@@ -6410,7 +6410,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>67</v>
       </c>
@@ -6421,7 +6421,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>109</v>
       </c>
@@ -6432,7 +6432,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>109</v>
       </c>
@@ -6443,7 +6443,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>36</v>
       </c>
@@ -6454,7 +6454,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>36</v>
       </c>
@@ -6465,7 +6465,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>36</v>
       </c>
@@ -6476,7 +6476,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>36</v>
       </c>
@@ -6487,7 +6487,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>36</v>
       </c>
@@ -6498,7 +6498,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>39</v>
       </c>
@@ -6509,7 +6509,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>39</v>
       </c>
@@ -6520,7 +6520,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>39</v>
       </c>
@@ -6531,7 +6531,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>39</v>
       </c>
@@ -6542,7 +6542,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>87</v>
       </c>
@@ -6553,7 +6553,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>87</v>
       </c>
@@ -6564,7 +6564,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>72</v>
       </c>
@@ -6575,7 +6575,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>69</v>
       </c>
@@ -6586,7 +6586,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>13</v>
       </c>
@@ -6597,7 +6597,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>83</v>
       </c>
@@ -6608,7 +6608,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>83</v>
       </c>
@@ -6619,7 +6619,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>83</v>
       </c>
@@ -6630,7 +6630,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>487</v>
       </c>
@@ -6641,7 +6641,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>487</v>
       </c>
@@ -6652,7 +6652,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>487</v>
       </c>
@@ -6663,7 +6663,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>55</v>
       </c>
@@ -6674,7 +6674,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>55</v>
       </c>
@@ -6685,7 +6685,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>330</v>
       </c>
@@ -6696,7 +6696,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>399</v>
       </c>
@@ -6707,7 +6707,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>399</v>
       </c>
@@ -6718,7 +6718,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>399</v>
       </c>
@@ -6729,7 +6729,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>397</v>
       </c>
@@ -6740,7 +6740,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>40</v>
       </c>
@@ -6751,7 +6751,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>40</v>
       </c>
@@ -6762,7 +6762,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>40</v>
       </c>
@@ -6773,7 +6773,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>92</v>
       </c>
@@ -6784,7 +6784,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>92</v>
       </c>
@@ -6795,7 +6795,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>92</v>
       </c>
@@ -6806,7 +6806,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>24</v>
       </c>
@@ -6817,7 +6817,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>42</v>
       </c>
@@ -6828,7 +6828,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>42</v>
       </c>
@@ -6839,7 +6839,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>42</v>
       </c>
@@ -6850,7 +6850,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>42</v>
       </c>
@@ -6861,7 +6861,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>42</v>
       </c>
@@ -6872,7 +6872,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>42</v>
       </c>
@@ -6883,7 +6883,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>42</v>
       </c>
@@ -6894,7 +6894,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>42</v>
       </c>
@@ -6905,7 +6905,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>42</v>
       </c>
@@ -6916,7 +6916,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>264</v>
       </c>
@@ -6927,7 +6927,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>264</v>
       </c>
@@ -6938,7 +6938,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>95</v>
       </c>
@@ -6949,7 +6949,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>95</v>
       </c>
@@ -6960,7 +6960,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>95</v>
       </c>
@@ -6971,7 +6971,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>458</v>
       </c>
@@ -6982,7 +6982,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>458</v>
       </c>
@@ -6993,7 +6993,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>458</v>
       </c>
@@ -7004,7 +7004,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="18" t="s">
         <v>100</v>
       </c>
@@ -7015,7 +7015,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="18" t="s">
         <v>20</v>
       </c>

</xml_diff>